<commit_message>
Draft results rewrite, FHY, input pyrite data
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaPYR_pH3/RaPYR_pH3 Equilibrated Data.xlsx
+++ b/Sorption Experiments/RaPYR_pH3/RaPYR_pH3 Equilibrated Data.xlsx
@@ -450,10 +450,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1.305</v>
+        <v>1.27366666666667</v>
       </c>
       <c r="C2">
-        <v>0.093264</v>
+        <v>0.09216252</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -461,10 +461,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1.75388888888889</v>
+        <v>1.74133333333333</v>
       </c>
       <c r="C3">
-        <v>0.108156481481481</v>
+        <v>0.107753706666667</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -472,10 +472,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1.25388888888889</v>
+        <v>1.251</v>
       </c>
       <c r="C4">
-        <v>0.0915338888888889</v>
+        <v>0.09139806</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -483,10 +483,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5.53</v>
+        <v>5.52033333333333</v>
       </c>
       <c r="C5">
-        <v>0.192075333333333</v>
+        <v>0.191886786666667</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -494,10 +494,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>4.82944444444444</v>
+        <v>4.83366666666667</v>
       </c>
       <c r="C6">
-        <v>0.179494351851852</v>
+        <v>0.17952238</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -505,10 +505,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5.16222222222222</v>
+        <v>5.088</v>
       </c>
       <c r="C7">
-        <v>0.185495851851852</v>
+        <v>0.1841856</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -516,10 +516,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>19.1822222222222</v>
+        <v>18.8956666666667</v>
       </c>
       <c r="C8">
-        <v>0.357428740740741</v>
+        <v>0.35486062</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -527,10 +527,10 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>19.6544444444444</v>
+        <v>19.5463333333333</v>
       </c>
       <c r="C9">
-        <v>0.361641777777778</v>
+        <v>0.360825313333333</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -538,10 +538,10 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>18.7688888888889</v>
+        <v>18.6393333333333</v>
       </c>
       <c r="C10">
-        <v>0.353480740740741</v>
+        <v>0.352656186666667</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -549,10 +549,10 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>37.5844444444444</v>
+        <v>37.508</v>
       </c>
       <c r="C11">
-        <v>0.499873111111111</v>
+        <v>0.49960656</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -560,10 +560,10 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>38.4577777777778</v>
+        <v>38.086</v>
       </c>
       <c r="C12">
-        <v>0.506360740740741</v>
+        <v>0.50349692</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -571,10 +571,10 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>38.315</v>
+        <v>38.2003333333333</v>
       </c>
       <c r="C13">
-        <v>0.505758</v>
+        <v>0.505008406666667</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -582,10 +582,10 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>90.675</v>
+        <v>90.1833333333333</v>
       </c>
       <c r="C14">
-        <v>0.779805</v>
+        <v>0.777380333333333</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -593,10 +593,10 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>93.7355555555555</v>
+        <v>93.4766666666667</v>
       </c>
       <c r="C15">
-        <v>0.790503185185185</v>
+        <v>0.788943066666667</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -604,10 +604,10 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>97.1477777777778</v>
+        <v>98.6423333333333</v>
       </c>
       <c r="C16">
-        <v>0.803088296296296</v>
+        <v>0.81083998</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -615,10 +615,10 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>191.199444444444</v>
+        <v>191.358</v>
       </c>
       <c r="C17">
-        <v>1.12807672222222</v>
+        <v>1.1290122</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -626,10 +626,10 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>191.256666666667</v>
+        <v>189.927666666667</v>
       </c>
       <c r="C18">
-        <v>1.12841433333333</v>
+        <v>1.12817034</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -637,10 +637,10 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>189.825</v>
+        <v>190.764666666667</v>
       </c>
       <c r="C19">
-        <v>1.126295</v>
+        <v>1.12932682666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>